<commit_message>
some sword world replays
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7185FE4A-D50F-0641-9574-A50621E264F9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E100FFF6-30CC-3B48-A63D-A4CB378D32CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t>year</t>
   </si>
@@ -240,6 +240,33 @@
   </si>
   <si>
     <t>The City Where the Devil Dances in the Dark</t>
+  </si>
+  <si>
+    <t>盗賊たちの狂詩曲ソード・ワールドRPGリプレイ集〈1〉</t>
+  </si>
+  <si>
+    <t>Rhapsody of Rogues: Sword World Replay 1</t>
+  </si>
+  <si>
+    <t>rhapsody_of_rogues.jpg</t>
+  </si>
+  <si>
+    <t>symphony_of_monsters.jpg</t>
+  </si>
+  <si>
+    <t>Symphony of Monsters: Sword World Replay 2</t>
+  </si>
+  <si>
+    <t>モンスターたちの交響曲ソード・ワールドRPGリプレイ集〈2〉</t>
+  </si>
+  <si>
+    <t>終わりなき即興曲ソード・ワールドRPGリプレイ集〈3〉</t>
+  </si>
+  <si>
+    <t>Endless Improvisation: Sword World Replay 3</t>
+  </si>
+  <si>
+    <t>endless_improvisation.jpg</t>
   </si>
 </sst>
 </file>
@@ -606,15 +633,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D430A7-E684-4C40-967F-9BBFE637BC2E}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="41.1640625" customWidth="1"/>
+    <col min="2" max="2" width="60.5" customWidth="1"/>
     <col min="3" max="3" width="42.1640625" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
     <col min="5" max="5" width="22.33203125" customWidth="1"/>
@@ -994,6 +1021,57 @@
         <v>66</v>
       </c>
     </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1989</v>
+      </c>
+      <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1990</v>
+      </c>
+      <c r="B24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C24" t="s">
+        <v>73</v>
+      </c>
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1991</v>
+      </c>
+      <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>77</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
another sword world item
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{959EFF4A-A78E-C247-A560-876B25721843}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318E471F-7EFA-9044-B12F-2BCBF8BA58FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="108">
   <si>
     <t>year</t>
   </si>
@@ -332,9 +332,6 @@
     <t>アドベンチャラーに任せとけ!―ソード・ワールドRPGリプレイ集 風雲ミラルゴ編〈2〉</t>
   </si>
   <si>
-    <t>Leave it to the Adventurer! Sword World Replay Collection 2</t>
-  </si>
-  <si>
     <t>アサシンをやりこめろ!―ソード・ワールドRPGリプレイ集 風雲ミラルゴ編〈1〉</t>
   </si>
   <si>
@@ -347,7 +344,19 @@
     <t>宝の地図に勇者が集う―ソード・ワールドRPGリプレイ集アンマント財宝編〈1〉</t>
   </si>
   <si>
-    <t>Heroes Gather at the Treasure Map: Sword World Replace Collection 1</t>
+    <t>hero_challenges_large_labyrinth.jpg</t>
+  </si>
+  <si>
+    <t>大迷宮に勇者が挑ソード・ワールドRPGリプレイ集アンマント財宝編2</t>
+  </si>
+  <si>
+    <t>A Hero Challenges a Large Labyrinth: Sword World Replay Collection 2</t>
+  </si>
+  <si>
+    <t>Heroes Gather at the Treasure Map: Sword World Replay Collection 1</t>
+  </si>
+  <si>
+    <t>Leave It To the Adventurer: Sword World Replay Collection 2</t>
   </si>
 </sst>
 </file>
@@ -714,10 +723,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D430A7-E684-4C40-967F-9BBFE637BC2E}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD34"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1260,10 +1269,10 @@
         <v>1996</v>
       </c>
       <c r="B32" t="s">
+        <v>99</v>
+      </c>
+      <c r="C32" t="s">
         <v>100</v>
-      </c>
-      <c r="C32" t="s">
-        <v>101</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
@@ -1280,7 +1289,7 @@
         <v>98</v>
       </c>
       <c r="C33" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
@@ -1294,16 +1303,33 @@
         <v>1997</v>
       </c>
       <c r="B34" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" t="s">
+        <v>106</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1998</v>
+      </c>
+      <c r="B35" t="s">
+        <v>104</v>
+      </c>
+      <c r="C35" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
         <v>103</v>
-      </c>
-      <c r="C34" t="s">
-        <v>104</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
-        <v>102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
move guide to another directory
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318E471F-7EFA-9044-B12F-2BCBF8BA58FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DE5806-5F58-324E-819F-BF7F165A01DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
   <si>
     <t>year</t>
   </si>
@@ -132,15 +132,6 @@
   </si>
   <si>
     <t>western_countries_world_guide.jpg</t>
-  </si>
-  <si>
-    <t>ロードス島ワールドガイド―ソード</t>
-  </si>
-  <si>
-    <t>Lodoss Island World Guide</t>
-  </si>
-  <si>
-    <t>lodoss_island_world_guide.jpg</t>
   </si>
   <si>
     <t>stone_giant_labyrinth.jpg</t>
@@ -723,10 +714,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D430A7-E684-4C40-967F-9BBFE637BC2E}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -909,19 +900,19 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1998</v>
+        <v>1989</v>
       </c>
       <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
         <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -943,36 +934,36 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" t="s">
         <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" t="s">
         <v>44</v>
-      </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" t="s">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -994,7 +985,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="B16" t="s">
         <v>48</v>
@@ -1011,19 +1002,19 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="B17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" t="s">
         <v>51</v>
-      </c>
-      <c r="C17" t="s">
-        <v>52</v>
-      </c>
-      <c r="D17" t="s">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1031,50 +1022,50 @@
         <v>1993</v>
       </c>
       <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
         <v>55</v>
       </c>
-      <c r="C18" t="s">
-        <v>56</v>
-      </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1993</v>
+        <v>1995</v>
       </c>
       <c r="B19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" t="s">
         <v>58</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1995</v>
+        <v>1997</v>
       </c>
       <c r="B20" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
         <v>60</v>
-      </c>
-      <c r="D20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1096,27 +1087,27 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1997</v>
+        <v>1989</v>
       </c>
       <c r="B22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" t="s">
         <v>67</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" t="s">
         <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>1989</v>
+        <v>1990</v>
       </c>
       <c r="B23" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
         <v>70</v>
@@ -1125,15 +1116,15 @@
         <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>1990</v>
+        <v>1991</v>
       </c>
       <c r="B24" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C24" t="s">
         <v>73</v>
@@ -1142,58 +1133,58 @@
         <v>7</v>
       </c>
       <c r="E24" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>1991</v>
+        <v>1992</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
         <v>7</v>
       </c>
       <c r="E25" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1992</v>
+        <v>1993</v>
       </c>
       <c r="B26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1993</v>
+        <v>1994</v>
       </c>
       <c r="B27" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C27" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1201,33 +1192,33 @@
         <v>1994</v>
       </c>
       <c r="B28" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" t="s">
         <v>90</v>
       </c>
-      <c r="C28" t="s">
-        <v>91</v>
-      </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>1994</v>
+        <v>1995</v>
       </c>
       <c r="B29" t="s">
+        <v>91</v>
+      </c>
+      <c r="C29" t="s">
         <v>92</v>
       </c>
-      <c r="C29" t="s">
-        <v>93</v>
-      </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1235,33 +1226,33 @@
         <v>1995</v>
       </c>
       <c r="B30" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C30" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1995</v>
+        <v>1996</v>
       </c>
       <c r="B31" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1269,67 +1260,50 @@
         <v>1996</v>
       </c>
       <c r="B32" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1996</v>
+        <v>1997</v>
       </c>
       <c r="B33" t="s">
+        <v>99</v>
+      </c>
+      <c r="C33" t="s">
+        <v>103</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
         <v>98</v>
-      </c>
-      <c r="C33" t="s">
-        <v>107</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>1997</v>
+        <v>1998</v>
       </c>
       <c r="B34" t="s">
+        <v>101</v>
+      </c>
+      <c r="C34" t="s">
         <v>102</v>
       </c>
-      <c r="C34" t="s">
-        <v>106</v>
-      </c>
       <c r="D34" t="s">
         <v>7</v>
       </c>
       <c r="E34" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>1998</v>
-      </c>
-      <c r="B35" t="s">
-        <v>104</v>
-      </c>
-      <c r="C35" t="s">
-        <v>105</v>
-      </c>
-      <c r="D35" t="s">
-        <v>7</v>
-      </c>
-      <c r="E35" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new sworld world image
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07DE5806-5F58-324E-819F-BF7F165A01DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7D4DB6-75A5-A447-86F1-00992A6FA41A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
   <si>
     <t>year</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>Leave It To the Adventurer: Sword World Replay Collection 2</t>
+  </si>
+  <si>
+    <t>sword_world_world_guide_alt.jpg</t>
   </si>
 </sst>
 </file>
@@ -714,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D430A7-E684-4C40-967F-9BBFE637BC2E}">
-  <dimension ref="A1:E34"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,36 +886,36 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>1989</v>
+        <v>1996</v>
       </c>
       <c r="B11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D11" t="s">
         <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -920,50 +923,50 @@
         <v>1989</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D12" t="s">
         <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D14" t="s">
         <v>7</v>
       </c>
       <c r="E14" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -971,50 +974,50 @@
         <v>1991</v>
       </c>
       <c r="B15" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>1992</v>
+        <v>1991</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D16" t="s">
         <v>7</v>
       </c>
       <c r="E16" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
         <v>7</v>
       </c>
       <c r="E17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1022,50 +1025,50 @@
         <v>1993</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D18" t="s">
         <v>7</v>
       </c>
       <c r="E18" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="B19" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D19" t="s">
         <v>7</v>
       </c>
       <c r="E19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>1997</v>
+        <v>1995</v>
       </c>
       <c r="B20" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="D20" t="s">
         <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1073,118 +1076,118 @@
         <v>1997</v>
       </c>
       <c r="B21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D21" t="s">
         <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>1989</v>
+        <v>1997</v>
       </c>
       <c r="B22" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D22" t="s">
         <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>1989</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>1990</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>71</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>70</v>
       </c>
-      <c r="D23" t="s">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24">
+    <row r="25" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>1991</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>72</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>73</v>
       </c>
-      <c r="D24" t="s">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" t="s">
         <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>1992</v>
-      </c>
-      <c r="B25" t="s">
-        <v>80</v>
-      </c>
-      <c r="C25" t="s">
-        <v>83</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D26" t="s">
         <v>7</v>
       </c>
       <c r="E26" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>1994</v>
+        <v>1993</v>
       </c>
       <c r="B27" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
         <v>7</v>
       </c>
       <c r="E27" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
@@ -1192,33 +1195,33 @@
         <v>1994</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C28" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="D28" t="s">
         <v>7</v>
       </c>
       <c r="E28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>1995</v>
+        <v>1994</v>
       </c>
       <c r="B29" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D29" t="s">
         <v>7</v>
       </c>
       <c r="E29" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1226,33 +1229,33 @@
         <v>1995</v>
       </c>
       <c r="B30" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="C30" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D30" t="s">
         <v>7</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>1996</v>
+        <v>1995</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
         <v>7</v>
       </c>
       <c r="E31" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -1260,49 +1263,66 @@
         <v>1996</v>
       </c>
       <c r="B32" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D32" t="s">
         <v>7</v>
       </c>
       <c r="E32" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>1997</v>
+        <v>1996</v>
       </c>
       <c r="B33" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D33" t="s">
         <v>7</v>
       </c>
       <c r="E33" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
+        <v>1997</v>
+      </c>
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>103</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
         <v>1998</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>101</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>102</v>
       </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D35" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" t="s">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sword world product type
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B7D4DB6-75A5-A447-86F1-00992A6FA41A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C54C7C-9D34-9F40-BE8E-2669E294CF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
   <si>
     <t>year</t>
   </si>
@@ -351,6 +351,21 @@
   </si>
   <si>
     <t>sword_world_world_guide_alt.jpg</t>
+  </si>
+  <si>
+    <t>product_type</t>
+  </si>
+  <si>
+    <t>rulebook</t>
+  </si>
+  <si>
+    <t>replay</t>
+  </si>
+  <si>
+    <t>supplement</t>
+  </si>
+  <si>
+    <t>scenario</t>
   </si>
 </sst>
 </file>
@@ -717,10 +732,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D430A7-E684-4C40-967F-9BBFE637BC2E}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,10 +743,11 @@
     <col min="2" max="2" width="77.6640625" customWidth="1"/>
     <col min="3" max="3" width="65.33203125" customWidth="1"/>
     <col min="4" max="4" width="21.5" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
+    <col min="5" max="5" width="36" customWidth="1"/>
+    <col min="6" max="6" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -747,8 +763,11 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1989</v>
       </c>
@@ -764,8 +783,11 @@
       <c r="E2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1990</v>
       </c>
@@ -781,8 +803,11 @@
       <c r="E3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1990</v>
       </c>
@@ -798,8 +823,11 @@
       <c r="E4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -815,8 +843,11 @@
       <c r="E5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1996</v>
       </c>
@@ -832,8 +863,11 @@
       <c r="E6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1997</v>
       </c>
@@ -849,8 +883,11 @@
       <c r="E7" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2004</v>
       </c>
@@ -866,8 +903,11 @@
       <c r="E8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1993</v>
       </c>
@@ -883,8 +923,11 @@
       <c r="E9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1993</v>
       </c>
@@ -900,8 +943,11 @@
       <c r="E10" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1996</v>
       </c>
@@ -917,8 +963,11 @@
       <c r="E11" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1989</v>
       </c>
@@ -934,8 +983,11 @@
       <c r="E12" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1989</v>
       </c>
@@ -951,8 +1003,11 @@
       <c r="E13" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1990</v>
       </c>
@@ -968,8 +1023,11 @@
       <c r="E14" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1991</v>
       </c>
@@ -985,8 +1043,11 @@
       <c r="E15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1991</v>
       </c>
@@ -1002,8 +1063,11 @@
       <c r="E16" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1992</v>
       </c>
@@ -1019,8 +1083,11 @@
       <c r="E17" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1993</v>
       </c>
@@ -1036,8 +1103,11 @@
       <c r="E18" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1993</v>
       </c>
@@ -1053,8 +1123,11 @@
       <c r="E19" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1995</v>
       </c>
@@ -1070,8 +1143,11 @@
       <c r="E20" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1997</v>
       </c>
@@ -1087,8 +1163,11 @@
       <c r="E21" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1997</v>
       </c>
@@ -1104,8 +1183,11 @@
       <c r="E22" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1989</v>
       </c>
@@ -1121,8 +1203,11 @@
       <c r="E23" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1990</v>
       </c>
@@ -1138,8 +1223,11 @@
       <c r="E24" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1991</v>
       </c>
@@ -1155,8 +1243,11 @@
       <c r="E25" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1992</v>
       </c>
@@ -1172,8 +1263,11 @@
       <c r="E26" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1993</v>
       </c>
@@ -1189,8 +1283,11 @@
       <c r="E27" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1994</v>
       </c>
@@ -1206,8 +1303,11 @@
       <c r="E28" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1994</v>
       </c>
@@ -1223,8 +1323,11 @@
       <c r="E29" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1995</v>
       </c>
@@ -1240,8 +1343,11 @@
       <c r="E30" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1995</v>
       </c>
@@ -1257,8 +1363,11 @@
       <c r="E31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1996</v>
       </c>
@@ -1274,8 +1383,11 @@
       <c r="E32" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1996</v>
       </c>
@@ -1291,8 +1403,11 @@
       <c r="E33" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1997</v>
       </c>
@@ -1308,8 +1423,11 @@
       <c r="E34" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1998</v>
       </c>
@@ -1324,6 +1442,9 @@
       </c>
       <c r="E35" t="s">
         <v>100</v>
+      </c>
+      <c r="F35" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sword world product codes
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1C54C7C-9D34-9F40-BE8E-2669E294CF59}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{F0D09655-F7C2-764C-BEA8-375115A035C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="18740" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="checklist" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="128">
   <si>
     <t>year</t>
   </si>
@@ -366,6 +366,57 @@
   </si>
   <si>
     <t>scenario</t>
+  </si>
+  <si>
+    <t>product_code</t>
+  </si>
+  <si>
+    <t>6-1</t>
+  </si>
+  <si>
+    <t>6-2</t>
+  </si>
+  <si>
+    <t>6-3</t>
+  </si>
+  <si>
+    <t>6-4</t>
+  </si>
+  <si>
+    <t>6-5</t>
+  </si>
+  <si>
+    <t>6-7</t>
+  </si>
+  <si>
+    <t>6-8</t>
+  </si>
+  <si>
+    <t>6-9</t>
+  </si>
+  <si>
+    <t>6-10</t>
+  </si>
+  <si>
+    <t>6-11</t>
+  </si>
+  <si>
+    <t>6-13</t>
+  </si>
+  <si>
+    <t>6-15</t>
+  </si>
+  <si>
+    <t>6-20</t>
+  </si>
+  <si>
+    <t>6-27</t>
+  </si>
+  <si>
+    <t>6-28</t>
+  </si>
+  <si>
+    <t>6-35</t>
   </si>
 </sst>
 </file>
@@ -415,9 +466,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +784,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D430A7-E684-4C40-967F-9BBFE637BC2E}">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -747,7 +799,7 @@
     <col min="6" max="6" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -766,8 +818,11 @@
       <c r="F1" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1989</v>
       </c>
@@ -786,8 +841,11 @@
       <c r="F2" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1990</v>
       </c>
@@ -806,8 +864,11 @@
       <c r="F3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1990</v>
       </c>
@@ -826,8 +887,11 @@
       <c r="F4" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1996</v>
       </c>
@@ -846,8 +910,11 @@
       <c r="F5" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1996</v>
       </c>
@@ -866,8 +933,9 @@
       <c r="F6" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1997</v>
       </c>
@@ -886,8 +954,11 @@
       <c r="F7" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2004</v>
       </c>
@@ -906,8 +977,9 @@
       <c r="F8" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1993</v>
       </c>
@@ -926,8 +998,9 @@
       <c r="F9" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1993</v>
       </c>
@@ -946,8 +1019,9 @@
       <c r="F10" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1996</v>
       </c>
@@ -966,8 +1040,9 @@
       <c r="F11" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1989</v>
       </c>
@@ -986,8 +1061,11 @@
       <c r="F12" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1989</v>
       </c>
@@ -1006,8 +1084,11 @@
       <c r="F13" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1990</v>
       </c>
@@ -1026,8 +1107,11 @@
       <c r="F14" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1991</v>
       </c>
@@ -1046,8 +1130,11 @@
       <c r="F15" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1991</v>
       </c>
@@ -1066,8 +1153,11 @@
       <c r="F16" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1992</v>
       </c>
@@ -1086,8 +1176,11 @@
       <c r="F17" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>1993</v>
       </c>
@@ -1106,8 +1199,11 @@
       <c r="F18" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>1993</v>
       </c>
@@ -1126,8 +1222,9 @@
       <c r="F19" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1995</v>
       </c>
@@ -1146,8 +1243,11 @@
       <c r="F20" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G20" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1997</v>
       </c>
@@ -1166,8 +1266,11 @@
       <c r="F21" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G21" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1997</v>
       </c>
@@ -1186,8 +1289,9 @@
       <c r="F22" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1989</v>
       </c>
@@ -1206,8 +1310,11 @@
       <c r="F23" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G23" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1990</v>
       </c>
@@ -1226,8 +1333,11 @@
       <c r="F24" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G24" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1991</v>
       </c>
@@ -1246,8 +1356,11 @@
       <c r="F25" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G25" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1992</v>
       </c>
@@ -1266,8 +1379,9 @@
       <c r="F26" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1993</v>
       </c>
@@ -1286,8 +1400,9 @@
       <c r="F27" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1994</v>
       </c>
@@ -1306,8 +1421,9 @@
       <c r="F28" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1994</v>
       </c>
@@ -1326,8 +1442,9 @@
       <c r="F29" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1995</v>
       </c>
@@ -1346,8 +1463,9 @@
       <c r="F30" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1995</v>
       </c>
@@ -1366,8 +1484,9 @@
       <c r="F31" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1996</v>
       </c>
@@ -1386,8 +1505,9 @@
       <c r="F32" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1996</v>
       </c>
@@ -1406,8 +1526,9 @@
       <c r="F33" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1997</v>
       </c>
@@ -1426,8 +1547,9 @@
       <c r="F34" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1998</v>
       </c>
@@ -1446,6 +1568,7 @@
       <c r="F35" t="s">
         <v>108</v>
       </c>
+      <c r="G35" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
sword world image fix
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37A9B8CF-53C1-A641-97F6-F365B60542F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1209EFDF-F194-C643-9E71-228D6BA85917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
@@ -788,9 +788,6 @@
     <t>Night Breakers Explosion!-Sword World RPG Adventure &lt;5&gt;</t>
   </si>
   <si>
-    <t>night_breakers_explosion.jpg</t>
-  </si>
-  <si>
     <t>novel</t>
   </si>
   <si>
@@ -819,6 +816,9 @@
   </si>
   <si>
     <t>mirror_country_war.jpg</t>
+  </si>
+  <si>
+    <t>night_breakers_explosion.jpeg</t>
   </si>
 </sst>
 </file>
@@ -1201,7 +1201,7 @@
   <dimension ref="A1:G76"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="F77" sqref="F77"/>
+      <selection activeCell="E74" sqref="E74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2702,7 +2702,7 @@
         <v>239</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
@@ -2722,7 +2722,7 @@
         <v>244</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
@@ -2742,7 +2742,7 @@
         <v>245</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
@@ -2762,7 +2762,7 @@
         <v>248</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
@@ -2779,10 +2779,10 @@
         <v>7</v>
       </c>
       <c r="E73" t="s">
+        <v>261</v>
+      </c>
+      <c r="F73" s="4" t="s">
         <v>251</v>
-      </c>
-      <c r="F73" s="4" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
@@ -2790,19 +2790,19 @@
         <v>1997</v>
       </c>
       <c r="B74" t="s">
+        <v>252</v>
+      </c>
+      <c r="C74" t="s">
         <v>253</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
+        <v>7</v>
+      </c>
+      <c r="E74" t="s">
         <v>254</v>
       </c>
-      <c r="D74" t="s">
-        <v>7</v>
-      </c>
-      <c r="E74" t="s">
-        <v>255</v>
-      </c>
       <c r="F74" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
@@ -2810,19 +2810,19 @@
         <v>1998</v>
       </c>
       <c r="B75" t="s">
+        <v>255</v>
+      </c>
+      <c r="C75" t="s">
+        <v>257</v>
+      </c>
+      <c r="D75" t="s">
+        <v>7</v>
+      </c>
+      <c r="E75" t="s">
         <v>256</v>
       </c>
-      <c r="C75" t="s">
-        <v>258</v>
-      </c>
-      <c r="D75" t="s">
-        <v>7</v>
-      </c>
-      <c r="E75" t="s">
-        <v>257</v>
-      </c>
       <c r="F75" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
@@ -2830,19 +2830,19 @@
         <v>1998</v>
       </c>
       <c r="B76" t="s">
+        <v>258</v>
+      </c>
+      <c r="C76" t="s">
         <v>259</v>
       </c>
-      <c r="C76" t="s">
+      <c r="D76" t="s">
+        <v>7</v>
+      </c>
+      <c r="E76" t="s">
         <v>260</v>
       </c>
-      <c r="D76" t="s">
-        <v>7</v>
-      </c>
-      <c r="E76" t="s">
-        <v>261</v>
-      </c>
       <c r="F76" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more sword world product codes
</commit_message>
<xml_diff>
--- a/sword-world/checklist.xlsx
+++ b/sword-world/checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clark/Local/src/weatherspud/japanese-collectors-list/sword-world/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{EE0FAC56-F9C7-504F-B98C-E2FDAF63B0C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CA8C2682-CB05-4749-B63F-A1760D8A8B76}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="26880" windowHeight="16340" xr2:uid="{40353CB1-C1C9-6644-9E02-3913D474AAB5}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="322">
   <si>
     <t>year</t>
   </si>
@@ -996,6 +996,9 @@
   </si>
   <si>
     <t>bablies_forever_2003.jpg</t>
+  </si>
+  <si>
+    <t>6-81</t>
   </si>
 </sst>
 </file>
@@ -1377,8 +1380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D430A7-E684-4C40-967F-9BBFE637BC2E}">
   <dimension ref="A1:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="B82" sqref="B82"/>
+    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2763,6 +2766,9 @@
       <c r="F61" s="4" t="s">
         <v>108</v>
       </c>
+      <c r="G61" s="2" t="s">
+        <v>321</v>
+      </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">

</xml_diff>